<commit_message>
Init project with data
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Documents/GitHub/GeoPressureTemplate/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Library/CloudStorage/Box-Box/WoodlandKingfisher/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52A1AAC-00FB-9A4B-8C2C-FEE87180D196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDFE119-8D18-FD4D-A2BE-F5E079146F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43860" yWindow="1740" windowWidth="31760" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tracks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Color</t>
   </si>
@@ -120,26 +120,41 @@
     <t>thr_dur</t>
   </si>
   <si>
-    <t>18LX</t>
-  </si>
-  <si>
-    <t>Great Reed Warbler</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
     <t>thr_prob_percentile</t>
   </si>
   <si>
     <t>thr_gs</t>
+  </si>
+  <si>
+    <t>16LN</t>
+  </si>
+  <si>
+    <t>16LO</t>
+  </si>
+  <si>
+    <t>16LP</t>
+  </si>
+  <si>
+    <t>20IK</t>
+  </si>
+  <si>
+    <t>22NO</t>
+  </si>
+  <si>
+    <t>Halcyon senegaloides</t>
+  </si>
+  <si>
+    <t>Woodland Kingfisher</t>
+  </si>
+  <si>
+    <t>kernel_adjust</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -297,6 +312,11 @@
       <color rgb="FFAD0000"/>
       <name val="Var(--bs-font-monospace)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -479,7 +499,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -594,6 +614,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -640,13 +688,20 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -693,21 +748,9 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
@@ -717,6 +760,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
@@ -781,13 +833,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AF2" totalsRowShown="0">
-  <autoFilter ref="A1:AF2" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AF6" totalsRowShown="0">
+  <autoFilter ref="A1:AF6" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
   <tableColumns count="32">
-    <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="13" dataCellStyle="Normal_Feuil1"/>
+    <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="12" dataCellStyle="Normal_Feuil1"/>
     <tableColumn id="38" xr3:uid="{5F80A124-B607-6D47-A8B2-B6EBC16D0EC2}" name="crop_start"/>
     <tableColumn id="39" xr3:uid="{C4B8ED7B-88BE-D143-A9A5-6213689753CA}" name="crop_end"/>
-    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="11"/>
     <tableColumn id="43" xr3:uid="{0ACC25F8-5611-FA4F-B49C-6E30F1D95C08}" name="extent_N"/>
     <tableColumn id="44" xr3:uid="{7341665D-D68F-3E48-95CE-8E270ED9FA6A}" name="extent_W"/>
     <tableColumn id="45" xr3:uid="{18F1D038-2D60-FF49-8711-16897DCC1A1A}" name="extent_S"/>
@@ -797,19 +849,19 @@
     <tableColumn id="49" xr3:uid="{A0BE4E97-52EA-C245-B384-C2C954FDB62B}" name="map_margin"/>
     <tableColumn id="50" xr3:uid="{98646B4B-4B26-0A4C-A7C3-1140DBCABB7B}" name="prob_map_s"/>
     <tableColumn id="51" xr3:uid="{AD7A8CAB-A777-7C4D-A6A2-601A4074FBB2}" name="prob_map_thr"/>
-    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="11"/>
+    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{596B01C4-C1D6-754D-830C-2EF105F617D0}" name="kernel_adjust"/>
     <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon"/>
     <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat"/>
-    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="8"/>
-    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="7"/>
-    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="6"/>
-    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{7EF3D097-7731-F44F-851D-98DEC75B75D2}" name="Column3" dataDxfId="0"/>
+    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="0"/>
+    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="9"/>
+    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="2"/>
+    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="8"/>
+    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="4"/>
     <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="RingNo" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name"/>
     <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name"/>
@@ -1118,22 +1170,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF13"/>
+  <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O1:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" customWidth="1"/>
-    <col min="16" max="16" width="18.83203125" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.1640625" customWidth="1"/>
-    <col min="20" max="20" width="14.1640625" customWidth="1"/>
-    <col min="21" max="26" width="17.33203125" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" customWidth="1"/>
+    <col min="22" max="26" width="17.33203125" customWidth="1"/>
     <col min="28" max="28" width="17.33203125" customWidth="1"/>
     <col min="29" max="29" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="20.5" bestFit="1" customWidth="1"/>
@@ -1189,40 +1242,40 @@
         <v>7</v>
       </c>
       <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>27</v>
       </c>
-      <c r="X1" t="s">
-        <v>32</v>
-      </c>
       <c r="Y1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Z1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA1" t="s">
         <v>2</v>
@@ -1244,29 +1297,29 @@
       </c>
     </row>
     <row r="2" spans="1:32">
-      <c r="A2" t="s">
-        <v>29</v>
+      <c r="A2" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="B2" s="1">
-        <v>42906</v>
+        <v>42776</v>
       </c>
       <c r="C2" s="1">
-        <v>43222</v>
-      </c>
-      <c r="D2" s="4">
-        <v>12</v>
+        <v>43079</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>-16</v>
+        <v>9</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>-33</v>
       </c>
       <c r="H2">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -1287,41 +1340,381 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>17.05</v>
+        <v>1.4</v>
       </c>
       <c r="P2">
-        <v>48.9</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>42906</v>
+        <v>28.768573249999999</v>
+      </c>
+      <c r="Q2">
+        <v>-22.724631630000001</v>
       </c>
       <c r="R2" s="1">
-        <v>42952</v>
-      </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
+        <v>42776</v>
+      </c>
+      <c r="S2" s="1">
+        <v>42830</v>
+      </c>
+      <c r="T2" s="1">
+        <v>43058</v>
+      </c>
+      <c r="U2" s="1">
+        <v>43079</v>
+      </c>
       <c r="V2" s="1"/>
-      <c r="W2" s="4">
+      <c r="W2" s="1"/>
+      <c r="X2" s="3">
         <v>0.1</v>
       </c>
-      <c r="X2" s="4">
+      <c r="Y2" s="3">
         <v>0.9</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="Z2" s="3">
         <v>120</v>
       </c>
-      <c r="Z2" s="4"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
       <c r="AC2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42745</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43092</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>-33</v>
+      </c>
+      <c r="H3">
+        <v>43</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>300</v>
+      </c>
+      <c r="K3">
         <v>30</v>
       </c>
-      <c r="AF2" s="2"/>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0.9</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1.4</v>
+      </c>
+      <c r="P3">
+        <v>28.771320169999999</v>
+      </c>
+      <c r="Q3">
+        <v>-22.720038580000001</v>
+      </c>
+      <c r="R3" s="1">
+        <v>42745</v>
+      </c>
+      <c r="S3" s="1">
+        <v>42820</v>
+      </c>
+      <c r="T3" s="1">
+        <v>43054</v>
+      </c>
+      <c r="U3" s="1">
+        <v>43092</v>
+      </c>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>120</v>
+      </c>
+      <c r="AA3" s="1"/>
+      <c r="AB3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="8" spans="1:32">
-      <c r="P8" s="3"/>
+    <row r="4" spans="1:32">
+      <c r="A4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42750</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43089</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>-33</v>
+      </c>
+      <c r="H4">
+        <v>43</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>300</v>
+      </c>
+      <c r="K4">
+        <v>30</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0.9</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1.4</v>
+      </c>
+      <c r="P4">
+        <v>28.76930617</v>
+      </c>
+      <c r="Q4">
+        <v>-22.720402889999999</v>
+      </c>
+      <c r="R4" s="1">
+        <v>42750</v>
+      </c>
+      <c r="S4" s="1">
+        <v>42840</v>
+      </c>
+      <c r="T4" s="1">
+        <v>43053</v>
+      </c>
+      <c r="U4" s="1">
+        <v>43089</v>
+      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>120</v>
+      </c>
+      <c r="AA4" s="1"/>
+      <c r="AB4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="13" spans="1:32">
-      <c r="H13" s="5"/>
+    <row r="5" spans="1:32">
+      <c r="A5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43088</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43451</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>-33</v>
+      </c>
+      <c r="H5">
+        <v>43</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>300</v>
+      </c>
+      <c r="K5">
+        <v>30</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0.9</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>1.4</v>
+      </c>
+      <c r="P5">
+        <v>28.7814561</v>
+      </c>
+      <c r="Q5">
+        <v>-22.7466829</v>
+      </c>
+      <c r="R5" s="1">
+        <v>43088</v>
+      </c>
+      <c r="S5" s="1">
+        <v>43182</v>
+      </c>
+      <c r="T5" s="1">
+        <v>43074</v>
+      </c>
+      <c r="U5" s="1">
+        <v>43451</v>
+      </c>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>120</v>
+      </c>
+      <c r="AA5" s="1"/>
+      <c r="AB5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32">
+      <c r="A6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43489</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43737</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>-33</v>
+      </c>
+      <c r="H6">
+        <v>43</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>300</v>
+      </c>
+      <c r="K6">
+        <v>30</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0.9</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>1.4</v>
+      </c>
+      <c r="P6">
+        <v>28.774911100000001</v>
+      </c>
+      <c r="Q6">
+        <v>-22.725408300000002</v>
+      </c>
+      <c r="R6" s="1">
+        <v>43489</v>
+      </c>
+      <c r="S6" s="1">
+        <v>43572</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>120</v>
+      </c>
+      <c r="AA6" s="8"/>
+      <c r="AB6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+    </row>
+    <row r="7" spans="1:32">
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="12" spans="1:32">
+      <c r="H12" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>